<commit_message>
Refactor with sonar lint
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Facultate\vvss\PizzaShop\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDA7EC9-1272-4929-A625-FA5D6D1608C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5944E1A-5B0F-4AF5-AFC7-6D8D4513EA8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18075" yWindow="4845" windowWidth="20745" windowHeight="12960" tabRatio="800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" tabRatio="800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="92">
   <si>
     <t>do not print this form</t>
   </si>
@@ -349,7 +349,55 @@
     <t>Buffer writer-ul nu este inchis in situatia in care la scrierea in fisier apare o eroare, nu este tratat cazul de finally.</t>
   </si>
   <si>
-    <t>C06</t>
+    <t>e.printStackTrace();</t>
+  </si>
+  <si>
+    <t>PaymentRepository.java, 68</t>
+  </si>
+  <si>
+    <t>logger.error(e);</t>
+  </si>
+  <si>
+    <t>Resources should be closed</t>
+  </si>
+  <si>
+    <t>Throwable.printStackTrace(...) should not be called</t>
+  </si>
+  <si>
+    <t>Standard outputs should not be used directly to log anything</t>
+  </si>
+  <si>
+    <t>try { br = new BufferedReader(new FileReader(file)); ..</t>
+  </si>
+  <si>
+    <t>try (BufferedReader br = new BufferedReader(new FileReader(file))) {</t>
+  </si>
+  <si>
+    <t>MenuRepository.java, 23</t>
+  </si>
+  <si>
+    <t>PaymentRepository.java, 63</t>
+  </si>
+  <si>
+    <t>System.out.println(p.toString());</t>
+  </si>
+  <si>
+    <t>logger.info(p.toString());</t>
+  </si>
+  <si>
+    <t>System.out.println("--------------------------");</t>
+  </si>
+  <si>
+    <t>KitchenGUIController.java, 59</t>
+  </si>
+  <si>
+    <t>KitchenGUIController.java, 60</t>
+  </si>
+  <si>
+    <t>System.out.println("Table " + extractedTableNumberInteger + " ready at: " + now.get(Calendar.HOUR) + ":" + now.get(Calendar.MINUTE));</t>
+  </si>
+  <si>
+    <t>Ignored, because it is meant to be part of the UI.</t>
   </si>
 </sst>
 </file>
@@ -514,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -543,6 +591,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -960,8 +1009,8 @@
   </sheetPr>
   <dimension ref="A1:AMK27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,19 +1031,19 @@
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
         <v>3</v>
@@ -1018,10 +1067,10 @@
       <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="24"/>
       <c r="H4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1036,10 +1085,10 @@
       <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="25"/>
       <c r="H5" s="4" t="s">
         <v>11</v>
       </c>
@@ -1051,15 +1100,15 @@
       <c r="C6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
@@ -1287,8 +1336,8 @@
   </sheetPr>
   <dimension ref="A1:AMK28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,19 +1357,19 @@
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
         <v>3</v>
@@ -1344,10 +1393,10 @@
       <c r="C4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="26"/>
       <c r="H4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1362,10 +1411,10 @@
       <c r="C5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="26"/>
+      <c r="E5" s="27"/>
       <c r="H5" s="4" t="s">
         <v>11</v>
       </c>
@@ -1377,15 +1426,15 @@
       <c r="C6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
@@ -1614,8 +1663,8 @@
   </sheetPr>
   <dimension ref="A1:AMK32"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,19 +1685,19 @@
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
         <v>3</v>
@@ -1672,10 +1721,10 @@
       <c r="C4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="H4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1690,10 +1739,10 @@
       <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="28"/>
+      <c r="E5" s="29"/>
       <c r="H5" s="4" t="s">
         <v>11</v>
       </c>
@@ -1705,15 +1754,15 @@
       <c r="C6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
@@ -1793,12 +1842,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>66</v>
-      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1953,7 +1998,9 @@
         <v>25</v>
       </c>
       <c r="D32" s="15"/>
-      <c r="E32" s="10"/>
+      <c r="E32" s="20">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1976,18 +2023,18 @@
   </sheetPr>
   <dimension ref="A1:AMK32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:J5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="56.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="50" style="1" customWidth="1"/>
+    <col min="6" max="6" width="37.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="1" customWidth="1"/>
     <col min="9" max="9" width="26.7109375" style="1" customWidth="1"/>
@@ -1999,19 +2046,19 @@
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
         <v>3</v>
@@ -2035,8 +2082,8 @@
       <c r="C4" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
       <c r="H4" s="4" t="s">
         <v>8</v>
       </c>
@@ -2051,8 +2098,8 @@
       <c r="C5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
       <c r="H5" s="4" t="s">
         <v>11</v>
       </c>
@@ -2064,8 +2111,8 @@
       <c r="C6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
@@ -2084,54 +2131,94 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>1</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
         <f t="shared" ref="B11:B30" si="0">B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="C11" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
+      <c r="C14" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
@@ -2297,11 +2384,11 @@
       <c r="E31" s="13"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
       <c r="F32" s="18"/>
     </row>
   </sheetData>
@@ -2314,6 +2401,6 @@
     <mergeCell ref="D6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add final sonar lint adjustments
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Facultate\vvss\PizzaShop\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5944E1A-5B0F-4AF5-AFC7-6D8D4513EA8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18430D9-AEDB-45ED-AA35-A505D9699B3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" tabRatio="800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="25305" windowHeight="13185" tabRatio="800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="1" r:id="rId1"/>
@@ -397,7 +397,7 @@
     <t>System.out.println("Table " + extractedTableNumberInteger + " ready at: " + now.get(Calendar.HOUR) + ":" + now.get(Calendar.MINUTE));</t>
   </si>
   <si>
-    <t>Ignored, because it is meant to be part of the UI.</t>
+    <t>Ignored, because it is meant to be part of the UI. ( is it? )</t>
   </si>
 </sst>
 </file>
@@ -2023,8 +2023,8 @@
   </sheetPr>
   <dimension ref="A1:AMK32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>